<commit_message>
Fixed client and contract error issues when the filed is empty or not find
</commit_message>
<xml_diff>
--- a/CONFIG/eLIMS_contract_analysis.xlsx
+++ b/CONFIG/eLIMS_contract_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELPV\ELPV_OCRTool\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118C76ED-F258-4E36-B503-CADABC79DBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4F2441-D2EC-4793-B62C-12278931940D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_contract" sheetId="1" r:id="rId1"/>
@@ -13932,7 +13932,7 @@
     <col min="1" max="1" width="23.54296875" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.81640625" customWidth="1"/>
     <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" customWidth="1"/>
     <col min="5" max="5" width="28.453125" customWidth="1"/>
     <col min="6" max="6" width="48.453125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>

</xml_diff>